<commit_message>
Migrated over to new method for CO2 evolutions, updating submodules to match, and saving temperature and d11B output separately.
</commit_message>
<xml_diff>
--- a/Trudgill_et_al_202X/Data/TJ_d11B.xlsx
+++ b/Trudgill_et_al_202X/Data/TJ_d11B.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ross\Documents\Work\Postdoc\St_Andrews\Output\Private_Papers\Trudgill_et_al_202X\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEA4C2A5-117B-40D1-8035-F092A3CD889C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61449F9E-F90D-44B4-8558-7235FAD6B7D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="2" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Original" sheetId="4" r:id="rId1"/>
     <sheet name="Reformatted" sheetId="1" r:id="rId2"/>
     <sheet name="With_Age" sheetId="5" r:id="rId3"/>
-    <sheet name="With_Temperature" sheetId="6" r:id="rId10"/>
+    <sheet name="Temperature_Calibrations" sheetId="6" r:id="rId4"/>
+    <sheet name="Delta_Temperature" sheetId="7" r:id="rId11"/>
   </sheets>
   <calcPr calcId="191029" fullCalcOnLoad="true"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="221">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="149">
   <si>
     <t>sample</t>
   </si>
@@ -258,9 +259,6 @@
     <t>LAV040</t>
   </si>
   <si>
-    <t>sample</t>
-  </si>
-  <si>
     <t>height</t>
   </si>
   <si>
@@ -273,355 +271,142 @@
     <t>d11B_uncertainty</t>
   </si>
   <si>
+    <t>d18O</t>
+  </si>
+  <si>
+    <t>d18O_uncertainty</t>
+  </si>
+  <si>
+    <t>d13C</t>
+  </si>
+  <si>
+    <t>d13C_uncertainty</t>
+  </si>
+  <si>
+    <t>oneil_temperature</t>
+  </si>
+  <si>
+    <t>oneil_temperature_uncertainty</t>
+  </si>
+  <si>
+    <t>kim_oneil_temperature</t>
+  </si>
+  <si>
+    <t>kim_oneil_temperature_uncertainty</t>
+  </si>
+  <si>
+    <t>hansen_temperature</t>
+  </si>
+  <si>
+    <t>hansen_temperature_uncertainty</t>
+  </si>
+  <si>
+    <t>anderson_arthur_temperature</t>
+  </si>
+  <si>
+    <t>anderson_arthur_temperature_uncertainty</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>Ma</t>
+  </si>
+  <si>
+    <t>‰</t>
+  </si>
+  <si>
+    <t>°C</t>
+  </si>
+  <si>
+    <t>height</t>
+  </si>
+  <si>
+    <t>age</t>
+  </si>
+  <si>
+    <t>d11B</t>
+  </si>
+  <si>
+    <t>d11B_uncertainty</t>
+  </si>
+  <si>
+    <t>d18O</t>
+  </si>
+  <si>
+    <t>d18O_uncertainty</t>
+  </si>
+  <si>
+    <t>d13C</t>
+  </si>
+  <si>
+    <t>d13C_uncertainty</t>
+  </si>
+  <si>
+    <t>oneil_temperature</t>
+  </si>
+  <si>
+    <t>oneil_temperature_uncertainty</t>
+  </si>
+  <si>
+    <t>kim_oneil_temperature</t>
+  </si>
+  <si>
+    <t>kim_oneil_temperature_uncertainty</t>
+  </si>
+  <si>
+    <t>hansen_temperature</t>
+  </si>
+  <si>
+    <t>hansen_temperature_uncertainty</t>
+  </si>
+  <si>
+    <t>anderson_arthur_temperature</t>
+  </si>
+  <si>
+    <t>anderson_arthur_temperature_uncertainty</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>Ma</t>
+  </si>
+  <si>
+    <t>‰</t>
+  </si>
+  <si>
+    <t>°C</t>
+  </si>
+  <si>
+    <t>height</t>
+  </si>
+  <si>
+    <t>age</t>
+  </si>
+  <si>
+    <t>d11B</t>
+  </si>
+  <si>
+    <t>d11B_uncertainty</t>
+  </si>
+  <si>
+    <t>d18O</t>
+  </si>
+  <si>
+    <t>d18O_uncertainty</t>
+  </si>
+  <si>
+    <t>d13C</t>
+  </si>
+  <si>
+    <t>d13C_uncertainty</t>
+  </si>
+  <si>
     <t>delta_temperature</t>
   </si>
   <si>
     <t>delta_temperature_uncertainty</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
-    <t>m</t>
-  </si>
-  <si>
-    <t>Ma</t>
-  </si>
-  <si>
-    <t>‰</t>
-  </si>
-  <si>
-    <t>°C</t>
-  </si>
-  <si>
-    <t>LAV007</t>
-  </si>
-  <si>
-    <t>LAV003</t>
-  </si>
-  <si>
-    <t>LAV002</t>
-  </si>
-  <si>
-    <t>LAV012</t>
-  </si>
-  <si>
-    <t>LAV011</t>
-  </si>
-  <si>
-    <t>LAV010</t>
-  </si>
-  <si>
-    <t>LAV014</t>
-  </si>
-  <si>
-    <t>LAV016</t>
-  </si>
-  <si>
-    <t>LAV019</t>
-  </si>
-  <si>
-    <t>LAV020</t>
-  </si>
-  <si>
-    <t>LAV037</t>
-  </si>
-  <si>
-    <t>LAV021</t>
-  </si>
-  <si>
-    <t>LAV029</t>
-  </si>
-  <si>
-    <t>LAV030</t>
-  </si>
-  <si>
-    <t>LAV031</t>
-  </si>
-  <si>
-    <t>LAV038</t>
-  </si>
-  <si>
-    <t>LAV022</t>
-  </si>
-  <si>
-    <t>LAV025</t>
-  </si>
-  <si>
-    <t>LAV023</t>
-  </si>
-  <si>
-    <t>LAV039</t>
-  </si>
-  <si>
-    <t>LAV041</t>
-  </si>
-  <si>
-    <t>LAV040</t>
-  </si>
-  <si>
-    <t>sample</t>
-  </si>
-  <si>
-    <t>height</t>
-  </si>
-  <si>
-    <t>age</t>
-  </si>
-  <si>
-    <t>d11B</t>
-  </si>
-  <si>
-    <t>d11B_uncertainty</t>
-  </si>
-  <si>
-    <t>d18O</t>
-  </si>
-  <si>
-    <t>d18O_uncertainty</t>
-  </si>
-  <si>
-    <t>d13C</t>
-  </si>
-  <si>
-    <t>d13C_uncertainty</t>
-  </si>
-  <si>
-    <t>delta_temperature</t>
-  </si>
-  <si>
-    <t>delta_temperature_uncertainty</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
-    <t>m</t>
-  </si>
-  <si>
-    <t>Ma</t>
-  </si>
-  <si>
-    <t>‰</t>
-  </si>
-  <si>
-    <t>°C</t>
-  </si>
-  <si>
-    <t>LAV007</t>
-  </si>
-  <si>
-    <t>LAV003</t>
-  </si>
-  <si>
-    <t>LAV002</t>
-  </si>
-  <si>
-    <t>LAV012</t>
-  </si>
-  <si>
-    <t>LAV011</t>
-  </si>
-  <si>
-    <t>LAV010</t>
-  </si>
-  <si>
-    <t>LAV014</t>
-  </si>
-  <si>
-    <t>LAV016</t>
-  </si>
-  <si>
-    <t>LAV019</t>
-  </si>
-  <si>
-    <t>LAV020</t>
-  </si>
-  <si>
-    <t>LAV037</t>
-  </si>
-  <si>
-    <t>LAV021</t>
-  </si>
-  <si>
-    <t>LAV029</t>
-  </si>
-  <si>
-    <t>LAV030</t>
-  </si>
-  <si>
-    <t>LAV031</t>
-  </si>
-  <si>
-    <t>LAV038</t>
-  </si>
-  <si>
-    <t>LAV022</t>
-  </si>
-  <si>
-    <t>LAV025</t>
-  </si>
-  <si>
-    <t>LAV023</t>
-  </si>
-  <si>
-    <t>LAV039</t>
-  </si>
-  <si>
-    <t>LAV041</t>
-  </si>
-  <si>
-    <t>LAV040</t>
-  </si>
-  <si>
-    <t>sample</t>
-  </si>
-  <si>
-    <t>height</t>
-  </si>
-  <si>
-    <t>age</t>
-  </si>
-  <si>
-    <t>d11B</t>
-  </si>
-  <si>
-    <t>d11B_uncertainty</t>
-  </si>
-  <si>
-    <t>d18O</t>
-  </si>
-  <si>
-    <t>d18O_uncertainty</t>
-  </si>
-  <si>
-    <t>d13C</t>
-  </si>
-  <si>
-    <t>d13C_uncertainty</t>
-  </si>
-  <si>
-    <t>delta_temperature</t>
-  </si>
-  <si>
-    <t>delta_temperature_uncertainty</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
-    <t>m</t>
-  </si>
-  <si>
-    <t>Ma</t>
-  </si>
-  <si>
-    <t>‰</t>
-  </si>
-  <si>
-    <t>°C</t>
-  </si>
-  <si>
-    <t>LAV007</t>
-  </si>
-  <si>
-    <t>LAV003</t>
-  </si>
-  <si>
-    <t>LAV002</t>
-  </si>
-  <si>
-    <t>LAV012</t>
-  </si>
-  <si>
-    <t>LAV011</t>
-  </si>
-  <si>
-    <t>LAV010</t>
-  </si>
-  <si>
-    <t>LAV014</t>
-  </si>
-  <si>
-    <t>LAV016</t>
-  </si>
-  <si>
-    <t>LAV019</t>
-  </si>
-  <si>
-    <t>LAV020</t>
-  </si>
-  <si>
-    <t>LAV037</t>
-  </si>
-  <si>
-    <t>LAV021</t>
-  </si>
-  <si>
-    <t>LAV029</t>
-  </si>
-  <si>
-    <t>LAV030</t>
-  </si>
-  <si>
-    <t>LAV031</t>
-  </si>
-  <si>
-    <t>LAV038</t>
-  </si>
-  <si>
-    <t>LAV022</t>
-  </si>
-  <si>
-    <t>LAV025</t>
-  </si>
-  <si>
-    <t>LAV023</t>
-  </si>
-  <si>
-    <t>LAV039</t>
-  </si>
-  <si>
-    <t>LAV041</t>
-  </si>
-  <si>
-    <t>LAV040</t>
-  </si>
-  <si>
-    <t>sample</t>
-  </si>
-  <si>
-    <t>height</t>
-  </si>
-  <si>
-    <t>age</t>
-  </si>
-  <si>
-    <t>d11B</t>
-  </si>
-  <si>
-    <t>d11B_uncertainty</t>
-  </si>
-  <si>
-    <t>d18O</t>
-  </si>
-  <si>
-    <t>d18O_uncertainty</t>
-  </si>
-  <si>
-    <t>d13C</t>
-  </si>
-  <si>
-    <t>d13C_uncertainty</t>
-  </si>
-  <si>
-    <t>delta_temperature</t>
-  </si>
-  <si>
-    <t>delta_temperature_uncertainty</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
   </si>
   <si>
     <t>m</t>
@@ -723,7 +508,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="17">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -738,20 +523,11 @@
     <border/>
     <border/>
     <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
@@ -760,15 +536,6 @@
     <xf numFmtId="22" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1842,7 +1609,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E68F4B3C-2083-4337-8469-4076B988F653}">
   <dimension ref="A1:D24"/>
   <sheetViews>
-    <sheetView tabSelected="true" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
@@ -2619,860 +2386,2018 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:P24"/>
+  <sheetViews>
+    <sheetView tabSelected="true" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="5.7109375" customWidth="true"/>
+    <col min="2" max="2" width="11.7109375" customWidth="true"/>
+    <col min="4" max="4" width="13.7109375" customWidth="true"/>
+    <col min="7" max="7" width="11.7109375" customWidth="true"/>
+    <col min="8" max="8" width="13.7109375" customWidth="true"/>
+    <col min="9" max="9" width="11.7109375" customWidth="true"/>
+    <col min="10" max="10" width="12.7109375" customWidth="true"/>
+    <col min="11" max="11" width="11.7109375" customWidth="true"/>
+    <col min="12" max="12" width="12.7109375" customWidth="true"/>
+    <col min="13" max="13" width="11.7109375" customWidth="true"/>
+    <col min="14" max="14" width="12.7109375" customWidth="true"/>
+    <col min="15" max="15" width="11.7109375" customWidth="true"/>
+    <col min="16" max="16" width="12.7109375" customWidth="true"/>
+    <col min="3" max="3" width="11.7109375" customWidth="true"/>
+    <col min="5" max="5" width="13.7109375" customWidth="true"/>
+    <col min="6" max="6" width="13.7109375" customWidth="true"/>
+  </cols>
+  <sheetData>
+    <row r="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="H1" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="I1" s="0" t="s">
+        <v>101</v>
+      </c>
+      <c r="J1" s="0" t="s">
+        <v>102</v>
+      </c>
+      <c r="K1" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="L1" s="0" t="s">
+        <v>104</v>
+      </c>
+      <c r="M1" s="0" t="s">
+        <v>105</v>
+      </c>
+      <c r="N1" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="O1" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="P1" s="0" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="2" x14ac:dyDescent="0.3">
+      <c r="A2" s="0" t="s">
+        <v>109</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>111</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>111</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>111</v>
+      </c>
+      <c r="F2" s="0" t="s">
+        <v>111</v>
+      </c>
+      <c r="G2" s="0" t="s">
+        <v>111</v>
+      </c>
+      <c r="H2" s="0" t="s">
+        <v>111</v>
+      </c>
+      <c r="I2" s="0" t="s">
+        <v>112</v>
+      </c>
+      <c r="J2" s="0" t="s">
+        <v>112</v>
+      </c>
+      <c r="K2" s="0" t="s">
+        <v>112</v>
+      </c>
+      <c r="L2" s="0" t="s">
+        <v>112</v>
+      </c>
+      <c r="M2" s="0" t="s">
+        <v>112</v>
+      </c>
+      <c r="N2" s="0" t="s">
+        <v>112</v>
+      </c>
+      <c r="O2" s="0" t="s">
+        <v>112</v>
+      </c>
+      <c r="P2" s="0" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="3" x14ac:dyDescent="0.3">
+      <c r="A3" s="0">
+        <v>12.190000000000001</v>
+      </c>
+      <c r="B3" s="0">
+        <v>201.52877606845385</v>
+      </c>
+      <c r="C3" s="0">
+        <v>10.01219720849093</v>
+      </c>
+      <c r="D3" s="0">
+        <v>0.14363301630762756</v>
+      </c>
+      <c r="E3" s="0">
+        <v>-0.13250000000000001</v>
+      </c>
+      <c r="F3" s="0">
+        <v>0.40917600125129522</v>
+      </c>
+      <c r="G3" s="0">
+        <v>3.2324999999999999</v>
+      </c>
+      <c r="H3" s="0">
+        <v>0.395084379173192</v>
+      </c>
+      <c r="I3" s="0">
+        <v>9.066844382550741</v>
+      </c>
+      <c r="J3" s="0">
+        <v>1.6423581217727818</v>
+      </c>
+      <c r="K3" s="0">
+        <v>8.8559249067701842</v>
+      </c>
+      <c r="L3" s="0">
+        <v>1.7953739105371873</v>
+      </c>
+      <c r="M3" s="0">
+        <v>12.529999999999999</v>
+      </c>
+      <c r="N3" s="0">
+        <v>1.6367040050051813</v>
+      </c>
+      <c r="O3" s="0">
+        <v>11.745016250000001</v>
+      </c>
+      <c r="P3" s="0">
+        <v>1.5627585036237193</v>
+      </c>
+    </row>
+    <row r="4" x14ac:dyDescent="0.3">
+      <c r="A4" s="0">
+        <v>13.59</v>
+      </c>
+      <c r="B4" s="0">
+        <v>201.48713504281281</v>
+      </c>
+      <c r="C4" s="0">
+        <v>10.24097362914215</v>
+      </c>
+      <c r="D4" s="0">
+        <v>0.11547829313839249</v>
+      </c>
+      <c r="E4" s="0">
+        <v>0.37744870533010322</v>
+      </c>
+      <c r="F4" s="0">
+        <v>0.77896182805958314</v>
+      </c>
+      <c r="G4" s="0">
+        <v>3.9028439203513017</v>
+      </c>
+      <c r="H4" s="0">
+        <v>0.50032627388643336</v>
+      </c>
+      <c r="I4" s="0">
+        <v>7.0568355841913348</v>
+      </c>
+      <c r="J4" s="0">
+        <v>3.0345941792290563</v>
+      </c>
+      <c r="K4" s="0">
+        <v>6.6484358894806981</v>
+      </c>
+      <c r="L4" s="0">
+        <v>3.3430377533865316</v>
+      </c>
+      <c r="M4" s="0">
+        <v>10.490205178679588</v>
+      </c>
+      <c r="N4" s="0">
+        <v>3.115847312238333</v>
+      </c>
+      <c r="O4" s="0">
+        <v>9.8543649408880984</v>
+      </c>
+      <c r="P4" s="0">
+        <v>2.8339935636573941</v>
+      </c>
+    </row>
+    <row r="5" x14ac:dyDescent="0.3">
+      <c r="A5" s="0">
+        <v>14.59</v>
+      </c>
+      <c r="B5" s="0">
+        <v>201.45739145306922</v>
+      </c>
+      <c r="C5" s="0">
+        <v>9.9763254692479073</v>
+      </c>
+      <c r="D5" s="0">
+        <v>0.10441689371381085</v>
+      </c>
+      <c r="E5" s="0">
+        <v>0.029023622047244513</v>
+      </c>
+      <c r="F5" s="0">
+        <v>0.8017221048052332</v>
+      </c>
+      <c r="G5" s="0">
+        <v>3.7846929133858254</v>
+      </c>
+      <c r="H5" s="0">
+        <v>0.51925427297230786</v>
+      </c>
+      <c r="I5" s="0">
+        <v>8.4054298846144029</v>
+      </c>
+      <c r="J5" s="0">
+        <v>3.1132944131159928</v>
+      </c>
+      <c r="K5" s="0">
+        <v>8.1366654403210337</v>
+      </c>
+      <c r="L5" s="0">
+        <v>3.4326203083304709</v>
+      </c>
+      <c r="M5" s="0">
+        <v>11.883905511811021</v>
+      </c>
+      <c r="N5" s="0">
+        <v>3.2068884192209333</v>
+      </c>
+      <c r="O5" s="0">
+        <v>11.108730766929133</v>
+      </c>
+      <c r="P5" s="0">
+        <v>2.901596591406459</v>
+      </c>
+    </row>
+    <row r="6" x14ac:dyDescent="0.3">
+      <c r="A6" s="0">
+        <v>15.02</v>
+      </c>
+      <c r="B6" s="0">
+        <v>201.44482068383846</v>
+      </c>
+      <c r="C6" s="0">
+        <v>10.878138239162579</v>
+      </c>
+      <c r="D6" s="0">
+        <v>0.10350965730875188</v>
+      </c>
+      <c r="E6" s="0">
+        <v>-0.70790171056203965</v>
+      </c>
+      <c r="F6" s="0">
+        <v>0.27775985316468221</v>
+      </c>
+      <c r="G6" s="0">
+        <v>4.5189615802335013</v>
+      </c>
+      <c r="H6" s="0">
+        <v>0.18251895219783656</v>
+      </c>
+      <c r="I6" s="0">
+        <v>11.417362722428514</v>
+      </c>
+      <c r="J6" s="0">
+        <v>1.1507301371662773</v>
+      </c>
+      <c r="K6" s="0">
+        <v>11.413364402077775</v>
+      </c>
+      <c r="L6" s="0">
+        <v>1.247338591423379</v>
+      </c>
+      <c r="M6" s="0">
+        <v>14.831606842248158</v>
+      </c>
+      <c r="N6" s="0">
+        <v>1.1110394126587284</v>
+      </c>
+      <c r="O6" s="0">
+        <v>14.001941725359753</v>
+      </c>
+      <c r="P6" s="0">
+        <v>1.1125962590266376</v>
+      </c>
+    </row>
+    <row r="7" x14ac:dyDescent="0.3">
+      <c r="A7" s="0">
+        <v>15.289999999999999</v>
+      </c>
+      <c r="B7" s="0">
+        <v>201.43974606845384</v>
+      </c>
+      <c r="C7" s="0">
+        <v>9.8872299810538102</v>
+      </c>
+      <c r="D7" s="0">
+        <v>0.10382787734144472</v>
+      </c>
+      <c r="E7" s="0">
+        <v>-0.8601732283464566</v>
+      </c>
+      <c r="F7" s="0">
+        <v>0.76956930410023416</v>
+      </c>
+      <c r="G7" s="0">
+        <v>3.7317440944881897</v>
+      </c>
+      <c r="H7" s="0">
+        <v>0.49856927291608044</v>
+      </c>
+      <c r="I7" s="0">
+        <v>12.045982916925004</v>
+      </c>
+      <c r="J7" s="0">
+        <v>2.9928755266293754</v>
+      </c>
+      <c r="K7" s="0">
+        <v>12.0954213844616</v>
+      </c>
+      <c r="L7" s="0">
+        <v>3.2985318139068247</v>
+      </c>
+      <c r="M7" s="0">
+        <v>15.440692913385826</v>
+      </c>
+      <c r="N7" s="0">
+        <v>3.0782772164009371</v>
+      </c>
+      <c r="O7" s="0">
+        <v>14.60878518503937</v>
+      </c>
+      <c r="P7" s="0">
+        <v>2.7918348112414737</v>
+      </c>
+    </row>
+    <row r="8" x14ac:dyDescent="0.3">
+      <c r="A8" s="0">
+        <v>15.640000000000001</v>
+      </c>
+      <c r="B8" s="0">
+        <v>201.43316786332562</v>
+      </c>
+      <c r="C8" s="0">
+        <v>10.708374995046363</v>
+      </c>
+      <c r="D8" s="0">
+        <v>0.10475773652306104</v>
+      </c>
+      <c r="E8" s="0">
+        <v>-0.71741309775302509</v>
+      </c>
+      <c r="F8" s="0">
+        <v>0.33941517159654622</v>
+      </c>
+      <c r="G8" s="0">
+        <v>3.7449907176237112</v>
+      </c>
+      <c r="H8" s="0">
+        <v>0.44666202463959798</v>
+      </c>
+      <c r="I8" s="0">
+        <v>11.455989173592044</v>
+      </c>
+      <c r="J8" s="0">
+        <v>1.3748282694110698</v>
+      </c>
+      <c r="K8" s="0">
+        <v>11.455462045671272</v>
+      </c>
+      <c r="L8" s="0">
+        <v>1.4989671504944593</v>
+      </c>
+      <c r="M8" s="0">
+        <v>14.869652391012099</v>
+      </c>
+      <c r="N8" s="0">
+        <v>1.3576606863861855</v>
+      </c>
+      <c r="O8" s="0">
+        <v>14.038945091543436</v>
+      </c>
+      <c r="P8" s="0">
+        <v>1.312898537245756</v>
+      </c>
+    </row>
+    <row r="9" x14ac:dyDescent="0.3">
+      <c r="A9" s="0">
+        <v>15.940000000000001</v>
+      </c>
+      <c r="B9" s="0">
+        <v>201.42752940178718</v>
+      </c>
+      <c r="C9" s="0">
+        <v>11.039549024903264</v>
+      </c>
+      <c r="D9" s="0">
+        <v>0.097150894309145294</v>
+      </c>
+      <c r="E9" s="0">
+        <v>0.063700787401571451</v>
+      </c>
+      <c r="F9" s="0">
+        <v>0.8017221048052332</v>
+      </c>
+      <c r="G9" s="0">
+        <v>4.077391304347822</v>
+      </c>
+      <c r="H9" s="0">
+        <v>0.51925427297230786</v>
+      </c>
+      <c r="I9" s="0">
+        <v>8.2798730366821864</v>
+      </c>
+      <c r="J9" s="0">
+        <v>3.1132944131159928</v>
+      </c>
+      <c r="K9" s="0">
+        <v>7.9953995799606368</v>
+      </c>
+      <c r="L9" s="0">
+        <v>3.4326203083304709</v>
+      </c>
+      <c r="M9" s="0">
+        <v>11.745196850393715</v>
+      </c>
+      <c r="N9" s="0">
+        <v>3.2068884192209333</v>
+      </c>
+      <c r="O9" s="0">
+        <v>10.99607180314962</v>
+      </c>
+      <c r="P9" s="0">
+        <v>2.901596591406459</v>
+      </c>
+    </row>
+    <row r="10" x14ac:dyDescent="0.3">
+      <c r="A10" s="0">
+        <v>16.190000000000001</v>
+      </c>
+      <c r="B10" s="0">
+        <v>201.42283068383844</v>
+      </c>
+      <c r="C10" s="0">
+        <v>10.762272249201416</v>
+      </c>
+      <c r="D10" s="0">
+        <v>0.088684907140420544</v>
+      </c>
+      <c r="E10" s="0">
+        <v>-1.1603550878255602</v>
+      </c>
+      <c r="F10" s="0">
+        <v>0.042883263899249804</v>
+      </c>
+      <c r="G10" s="0">
+        <v>3.3930330102967901</v>
+      </c>
+      <c r="H10" s="0">
+        <v>0.11008374535465781</v>
+      </c>
+      <c r="I10" s="0">
+        <v>13.307659375675012</v>
+      </c>
+      <c r="J10" s="0">
+        <v>0.18137757356371439</v>
+      </c>
+      <c r="K10" s="0">
+        <v>13.45767173761687</v>
+      </c>
+      <c r="L10" s="0">
+        <v>0.1954985620930586</v>
+      </c>
+      <c r="M10" s="0">
+        <v>16.641420351302241</v>
+      </c>
+      <c r="N10" s="0">
+        <v>0.1715330555969995</v>
+      </c>
+      <c r="O10" s="0">
+        <v>15.83630009410963</v>
+      </c>
+      <c r="P10" s="0">
+        <v>0.17691608859622798</v>
+      </c>
+    </row>
+    <row r="11" x14ac:dyDescent="0.3">
+      <c r="A11" s="0">
+        <v>16.539999999999999</v>
+      </c>
+      <c r="B11" s="0">
+        <v>201.41625247871025</v>
+      </c>
+      <c r="C11" s="0">
+        <v>10.835984879209818</v>
+      </c>
+      <c r="D11" s="0">
+        <v>0.10998966327131669</v>
+      </c>
+      <c r="E11" s="0">
+        <v>-0.63608858267716772</v>
+      </c>
+      <c r="F11" s="0">
+        <v>0.57102014147248525</v>
+      </c>
+      <c r="G11" s="0">
+        <v>3.2646003937007873</v>
+      </c>
+      <c r="H11" s="0">
+        <v>0.40554424135375533</v>
+      </c>
+      <c r="I11" s="0">
+        <v>11.12831663552199</v>
+      </c>
+      <c r="J11" s="0">
+        <v>2.2228820991431872</v>
+      </c>
+      <c r="K11" s="0">
+        <v>11.097540732692101</v>
+      </c>
+      <c r="L11" s="0">
+        <v>2.4492265208312922</v>
+      </c>
+      <c r="M11" s="0">
+        <v>14.544354330708671</v>
+      </c>
+      <c r="N11" s="0">
+        <v>2.2840805658899415</v>
+      </c>
+      <c r="O11" s="0">
+        <v>13.726067902952765</v>
+      </c>
+      <c r="P11" s="0">
+        <v>2.0746040556873755</v>
+      </c>
+    </row>
+    <row r="12" x14ac:dyDescent="0.3">
+      <c r="A12" s="0">
+        <v>16.890000000000001</v>
+      </c>
+      <c r="B12" s="0">
+        <v>201.40967427358206</v>
+      </c>
+      <c r="C12" s="0">
+        <v>10.459512485805641</v>
+      </c>
+      <c r="D12" s="0">
+        <v>0.11454452430566182</v>
+      </c>
+      <c r="E12" s="0">
+        <v>-0.11602362204725768</v>
+      </c>
+      <c r="F12" s="0">
+        <v>0.26972275316592836</v>
+      </c>
+      <c r="G12" s="0">
+        <v>3.4375554760200258</v>
+      </c>
+      <c r="H12" s="0">
+        <v>0.026115763878443478</v>
+      </c>
+      <c r="I12" s="0">
+        <v>8.994914023538545</v>
+      </c>
+      <c r="J12" s="0">
+        <v>1.0872424186522183</v>
+      </c>
+      <c r="K12" s="0">
+        <v>8.7789615187988677</v>
+      </c>
+      <c r="L12" s="0">
+        <v>1.1872196587642214</v>
+      </c>
+      <c r="M12" s="0">
+        <v>12.46409448818903</v>
+      </c>
+      <c r="N12" s="0">
+        <v>1.0788910126637137</v>
+      </c>
+      <c r="O12" s="0">
+        <v>11.673474084108861</v>
+      </c>
+      <c r="P12" s="0">
+        <v>1.0370672416197542</v>
+      </c>
+    </row>
+    <row r="13" x14ac:dyDescent="0.3">
+      <c r="A13" s="0">
+        <v>17.120000000000001</v>
+      </c>
+      <c r="B13" s="0">
+        <v>201.40535145306922</v>
+      </c>
+      <c r="C13" s="0">
+        <v>10.384159531398856</v>
+      </c>
+      <c r="D13" s="0">
+        <v>0.11901469625718146</v>
+      </c>
+      <c r="E13" s="0">
+        <v>-0.64282955071792613</v>
+      </c>
+      <c r="F13" s="0">
+        <v>0.057459940335953731</v>
+      </c>
+      <c r="G13" s="0">
+        <v>2.9475636868920798</v>
+      </c>
+      <c r="H13" s="0">
+        <v>0.13920006295401072</v>
+      </c>
+      <c r="I13" s="0">
+        <v>11.148319388693178</v>
+      </c>
+      <c r="J13" s="0">
+        <v>0.23855254630754258</v>
+      </c>
+      <c r="K13" s="0">
+        <v>11.121560222882529</v>
+      </c>
+      <c r="L13" s="0">
+        <v>0.25842676482810767</v>
+      </c>
+      <c r="M13" s="0">
+        <v>14.571318202871705</v>
+      </c>
+      <c r="N13" s="0">
+        <v>0.2298397613438149</v>
+      </c>
+      <c r="O13" s="0">
+        <v>13.741985722487271</v>
+      </c>
+      <c r="P13" s="0">
+        <v>0.23083276055806967</v>
+      </c>
+    </row>
+    <row r="14" x14ac:dyDescent="0.3">
+      <c r="A14" s="0">
+        <v>17.490000000000002</v>
+      </c>
+      <c r="B14" s="0">
+        <v>201.39839735050512</v>
+      </c>
+      <c r="C14" s="0">
+        <v>9.9436806178566286</v>
+      </c>
+      <c r="D14" s="0">
+        <v>0.096262499948600366</v>
+      </c>
+      <c r="E14" s="0">
+        <v>-0.98800293345685053</v>
+      </c>
+      <c r="F14" s="0">
+        <v>0.08750534568451096</v>
+      </c>
+      <c r="G14" s="0">
+        <v>2.9854948278524009</v>
+      </c>
+      <c r="H14" s="0">
+        <v>0.11011667130346764</v>
+      </c>
+      <c r="I14" s="0">
+        <v>12.587106030169805</v>
+      </c>
+      <c r="J14" s="0">
+        <v>0.36853730525503881</v>
+      </c>
+      <c r="K14" s="0">
+        <v>12.678553540315015</v>
+      </c>
+      <c r="L14" s="0">
+        <v>0.39768855372287526</v>
+      </c>
+      <c r="M14" s="0">
+        <v>15.952011733827398</v>
+      </c>
+      <c r="N14" s="0">
+        <v>0.35002138273804345</v>
+      </c>
+      <c r="O14" s="0">
+        <v>15.136858482901047</v>
+      </c>
+      <c r="P14" s="0">
+        <v>0.35883204408151481</v>
+      </c>
+    </row>
+    <row r="15" x14ac:dyDescent="0.3">
+      <c r="A15" s="0">
+        <v>18.210000000000001</v>
+      </c>
+      <c r="B15" s="0">
+        <v>201.38486504281281</v>
+      </c>
+      <c r="C15" s="0">
+        <v>9.9960501404771449</v>
+      </c>
+      <c r="D15" s="0">
+        <v>0.10589632985968327</v>
+      </c>
+      <c r="E15" s="0">
+        <v>-0.72329651716043897</v>
+      </c>
+      <c r="F15" s="0">
+        <v>0.7342202138225592</v>
+      </c>
+      <c r="G15" s="0">
+        <v>2.4119468375309268</v>
+      </c>
+      <c r="H15" s="0">
+        <v>0.49269297196336881</v>
+      </c>
+      <c r="I15" s="0">
+        <v>11.476810784760378</v>
+      </c>
+      <c r="J15" s="0">
+        <v>2.8517781093732615</v>
+      </c>
+      <c r="K15" s="0">
+        <v>11.479074269201325</v>
+      </c>
+      <c r="L15" s="0">
+        <v>3.1440967149077159</v>
+      </c>
+      <c r="M15" s="0">
+        <v>14.893186068641755</v>
+      </c>
+      <c r="N15" s="0">
+        <v>2.9368808552902372</v>
+      </c>
+      <c r="O15" s="0">
+        <v>14.057514483223082</v>
+      </c>
+      <c r="P15" s="0">
+        <v>2.6581892472327247</v>
+      </c>
+    </row>
+    <row r="16" x14ac:dyDescent="0.3">
+      <c r="A16" s="0">
+        <v>18.439999999999998</v>
+      </c>
+      <c r="B16" s="0">
+        <v>201.38054222229999</v>
+      </c>
+      <c r="C16" s="0">
+        <v>8.9507559822158029</v>
+      </c>
+      <c r="D16" s="0">
+        <v>0.20756565956142378</v>
+      </c>
+      <c r="E16" s="0">
+        <v>-0.76907473196726461</v>
+      </c>
+      <c r="F16" s="0">
+        <v>0.6414142290289524</v>
+      </c>
+      <c r="G16" s="0">
+        <v>2.3596288777516983</v>
+      </c>
+      <c r="H16" s="0">
+        <v>0.45617476985601274</v>
+      </c>
+      <c r="I16" s="0">
+        <v>11.668164265947521</v>
+      </c>
+      <c r="J16" s="0">
+        <v>2.4922285063161014</v>
+      </c>
+      <c r="K16" s="0">
+        <v>11.685992271957904</v>
+      </c>
+      <c r="L16" s="0">
+        <v>2.7474157355457907</v>
+      </c>
+      <c r="M16" s="0">
+        <v>15.076298927869059</v>
+      </c>
+      <c r="N16" s="0">
+        <v>2.5656569161158091</v>
+      </c>
+      <c r="O16" s="0">
+        <v>14.24326077884632</v>
+      </c>
+      <c r="P16" s="0">
+        <v>2.3235370181886816</v>
+      </c>
+    </row>
+    <row r="17" x14ac:dyDescent="0.3">
+      <c r="A17" s="0">
+        <v>18.84</v>
+      </c>
+      <c r="B17" s="0">
+        <v>201.37302427358205</v>
+      </c>
+      <c r="C17" s="0">
+        <v>9.2453681244467258</v>
+      </c>
+      <c r="D17" s="0">
+        <v>0.1085995457562766</v>
+      </c>
+      <c r="E17" s="0">
+        <v>-0.84868901858783219</v>
+      </c>
+      <c r="F17" s="0">
+        <v>0.48001251634441555</v>
+      </c>
+      <c r="G17" s="0">
+        <v>2.2686411216139062</v>
+      </c>
+      <c r="H17" s="0">
+        <v>0.39266485314756605</v>
+      </c>
+      <c r="I17" s="0">
+        <v>12.000952928881686</v>
+      </c>
+      <c r="J17" s="0">
+        <v>1.8669248488253749</v>
+      </c>
+      <c r="K17" s="0">
+        <v>12.045849668056309</v>
+      </c>
+      <c r="L17" s="0">
+        <v>2.0575357714380815</v>
+      </c>
+      <c r="M17" s="0">
+        <v>15.39475607435133</v>
+      </c>
+      <c r="N17" s="0">
+        <v>1.9200500653776615</v>
+      </c>
+      <c r="O17" s="0">
+        <v>14.56629781471282</v>
+      </c>
+      <c r="P17" s="0">
+        <v>1.741533141590335</v>
+      </c>
+    </row>
+    <row r="18" x14ac:dyDescent="0.3">
+      <c r="A18" s="0">
+        <v>20.140000000000001</v>
+      </c>
+      <c r="B18" s="0">
+        <v>201.34857658127436</v>
+      </c>
+      <c r="C18" s="0">
+        <v>8.1044394762742993</v>
+      </c>
+      <c r="D18" s="0">
+        <v>0.11800414700884421</v>
+      </c>
+      <c r="E18" s="0">
+        <v>-1.7484999999999999</v>
+      </c>
+      <c r="F18" s="0">
+        <v>0.8017221048052332</v>
+      </c>
+      <c r="G18" s="0">
+        <v>2.0686249999999999</v>
+      </c>
+      <c r="H18" s="0">
+        <v>0.51925427297230786</v>
+      </c>
+      <c r="I18" s="0">
+        <v>15.830597964332954</v>
+      </c>
+      <c r="J18" s="0">
+        <v>3.1132944131159928</v>
+      </c>
+      <c r="K18" s="0">
+        <v>16.166389151693803</v>
+      </c>
+      <c r="L18" s="0">
+        <v>3.4326203083304709</v>
+      </c>
+      <c r="M18" s="0">
+        <v>18.994</v>
+      </c>
+      <c r="N18" s="0">
+        <v>3.2068884192209333</v>
+      </c>
+      <c r="O18" s="0">
+        <v>18.309935599999999</v>
+      </c>
+      <c r="P18" s="0">
+        <v>2.901596591406459</v>
+      </c>
+    </row>
+    <row r="19" x14ac:dyDescent="0.3">
+      <c r="A19" s="0">
+        <v>20.640000000000001</v>
+      </c>
+      <c r="B19" s="0">
+        <v>201.33912786332564</v>
+      </c>
+      <c r="C19" s="0">
+        <v>9.7067607134899703</v>
+      </c>
+      <c r="D19" s="0">
+        <v>0.10902200739197236</v>
+      </c>
+      <c r="E19" s="0">
+        <v>-0.85450000000000126</v>
+      </c>
+      <c r="F19" s="0">
+        <v>0.68732639542481855</v>
+      </c>
+      <c r="G19" s="0">
+        <v>1.8960285714285714</v>
+      </c>
+      <c r="H19" s="0">
+        <v>0.2972487690582083</v>
+      </c>
+      <c r="I19" s="0">
+        <v>12.064091213708892</v>
+      </c>
+      <c r="J19" s="0">
+        <v>2.7755615653181813</v>
+      </c>
+      <c r="K19" s="0">
+        <v>12.102661732022582</v>
+      </c>
+      <c r="L19" s="0">
+        <v>3.0287884099805154</v>
+      </c>
+      <c r="M19" s="0">
+        <v>15.418000000000005</v>
+      </c>
+      <c r="N19" s="0">
+        <v>2.7493055816992737</v>
+      </c>
+      <c r="O19" s="0">
+        <v>14.643684110000004</v>
+      </c>
+      <c r="P19" s="0">
+        <v>2.646974494847087</v>
+      </c>
+    </row>
+    <row r="20" x14ac:dyDescent="0.3">
+      <c r="A20" s="0">
+        <v>21.120000000000001</v>
+      </c>
+      <c r="B20" s="0">
+        <v>201.33005709409485</v>
+      </c>
+      <c r="C20" s="0">
+        <v>8.4942813608424057</v>
+      </c>
+      <c r="D20" s="0">
+        <v>0.10853455716108885</v>
+      </c>
+      <c r="E20" s="0">
+        <v>-0.67841044776119386</v>
+      </c>
+      <c r="F20" s="0">
+        <v>0.54644398504411484</v>
+      </c>
+      <c r="G20" s="0">
+        <v>1.8858228855721393</v>
+      </c>
+      <c r="H20" s="0">
+        <v>0.26850920262175043</v>
+      </c>
+      <c r="I20" s="0">
+        <v>11.312683786521912</v>
+      </c>
+      <c r="J20" s="0">
+        <v>2.2550569005329986</v>
+      </c>
+      <c r="K20" s="0">
+        <v>11.294772749187629</v>
+      </c>
+      <c r="L20" s="0">
+        <v>2.4468829489450399</v>
+      </c>
+      <c r="M20" s="0">
+        <v>14.713641791044775</v>
+      </c>
+      <c r="N20" s="0">
+        <v>2.1857759401764585</v>
+      </c>
+      <c r="O20" s="0">
+        <v>13.908487989601987</v>
+      </c>
+      <c r="P20" s="0">
+        <v>2.1760041691617378</v>
+      </c>
+    </row>
+    <row r="21" x14ac:dyDescent="0.3">
+      <c r="A21" s="0">
+        <v>21.140000000000001</v>
+      </c>
+      <c r="B21" s="0">
+        <v>201.32967914537693</v>
+      </c>
+      <c r="C21" s="0">
+        <v>6.9697748282639225</v>
+      </c>
+      <c r="D21" s="0">
+        <v>0.087536853144447743</v>
+      </c>
+      <c r="E21" s="0">
+        <v>-0.68929104477611902</v>
+      </c>
+      <c r="F21" s="0">
+        <v>0.539983748256045</v>
+      </c>
+      <c r="G21" s="0">
+        <v>1.887542288557214</v>
+      </c>
+      <c r="H21" s="0">
+        <v>0.27226304613143282</v>
+      </c>
+      <c r="I21" s="0">
+        <v>11.357860748368532</v>
+      </c>
+      <c r="J21" s="0">
+        <v>2.2290211662200674</v>
+      </c>
+      <c r="K21" s="0">
+        <v>11.343710949358005</v>
+      </c>
+      <c r="L21" s="0">
+        <v>2.4184462805801683</v>
+      </c>
+      <c r="M21" s="0">
+        <v>14.757164179104475</v>
+      </c>
+      <c r="N21" s="0">
+        <v>2.1599349930241791</v>
+      </c>
+      <c r="O21" s="0">
+        <v>13.952199057960197</v>
+      </c>
+      <c r="P21" s="0">
+        <v>2.1511449651938892</v>
+      </c>
+    </row>
+    <row r="22" x14ac:dyDescent="0.3">
+      <c r="A22" s="0">
+        <v>23.539999999999999</v>
+      </c>
+      <c r="B22" s="0">
+        <v>201.28432529922307</v>
+      </c>
+      <c r="C22" s="0">
+        <v>7.1065964233074652</v>
+      </c>
+      <c r="D22" s="0">
+        <v>0.095202654485499486</v>
+      </c>
+      <c r="E22" s="0">
+        <v>-1.513714285714286</v>
+      </c>
+      <c r="F22" s="0">
+        <v>0.8017221048052332</v>
+      </c>
+      <c r="G22" s="0">
+        <v>2.722</v>
+      </c>
+      <c r="H22" s="0">
+        <v>0.51925427297230786</v>
+      </c>
+      <c r="I22" s="0">
+        <v>14.815279624824971</v>
+      </c>
+      <c r="J22" s="0">
+        <v>3.1132944131159928</v>
+      </c>
+      <c r="K22" s="0">
+        <v>15.07875347134283</v>
+      </c>
+      <c r="L22" s="0">
+        <v>3.4326203083304709</v>
+      </c>
+      <c r="M22" s="0">
+        <v>18.054857142857145</v>
+      </c>
+      <c r="N22" s="0">
+        <v>3.2068884192209333</v>
+      </c>
+      <c r="O22" s="0">
+        <v>17.311656057142855</v>
+      </c>
+      <c r="P22" s="0">
+        <v>2.901596591406459</v>
+      </c>
+    </row>
+    <row r="23" x14ac:dyDescent="0.3">
+      <c r="A23" s="0">
+        <v>23.890000000000001</v>
+      </c>
+      <c r="B23" s="0">
+        <v>201.27771119665897</v>
+      </c>
+      <c r="C23" s="0">
+        <v>9.3714561608127696</v>
+      </c>
+      <c r="D23" s="0">
+        <v>0.12036219998484181</v>
+      </c>
+      <c r="E23" s="0">
+        <v>-1.4951517857142858</v>
+      </c>
+      <c r="F23" s="0">
+        <v>0.8017221048052332</v>
+      </c>
+      <c r="G23" s="0">
+        <v>2.698375</v>
+      </c>
+      <c r="H23" s="0">
+        <v>0.51925427297230786</v>
+      </c>
+      <c r="I23" s="0">
+        <v>14.735613833354755</v>
+      </c>
+      <c r="J23" s="0">
+        <v>3.1132944131159928</v>
+      </c>
+      <c r="K23" s="0">
+        <v>14.993232037857201</v>
+      </c>
+      <c r="L23" s="0">
+        <v>3.4326203083304709</v>
+      </c>
+      <c r="M23" s="0">
+        <v>17.980607142857142</v>
+      </c>
+      <c r="N23" s="0">
+        <v>3.2068884192209333</v>
+      </c>
+      <c r="O23" s="0">
+        <v>17.233528350892854</v>
+      </c>
+      <c r="P23" s="0">
+        <v>2.901596591406459</v>
+      </c>
+    </row>
+    <row r="24" x14ac:dyDescent="0.3">
+      <c r="A24" s="0">
+        <v>24.189999999999998</v>
+      </c>
+      <c r="B24" s="0">
+        <v>201.27204196588974</v>
+      </c>
+      <c r="C24" s="0">
+        <v>9.5039834385630684</v>
+      </c>
+      <c r="D24" s="0">
+        <v>0.11997061322388737</v>
+      </c>
+      <c r="E24" s="0">
+        <v>-1.4792410714285715</v>
+      </c>
+      <c r="F24" s="0">
+        <v>0.8017221048052332</v>
+      </c>
+      <c r="G24" s="0">
+        <v>2.6781250000000001</v>
+      </c>
+      <c r="H24" s="0">
+        <v>0.51925427297230786</v>
+      </c>
+      <c r="I24" s="0">
+        <v>14.66732886923743</v>
+      </c>
+      <c r="J24" s="0">
+        <v>3.1132944131159928</v>
+      </c>
+      <c r="K24" s="0">
+        <v>14.919927952012378</v>
+      </c>
+      <c r="L24" s="0">
+        <v>3.4326203083304709</v>
+      </c>
+      <c r="M24" s="0">
+        <v>17.916964285714286</v>
+      </c>
+      <c r="N24" s="0">
+        <v>3.2068884192209333</v>
+      </c>
+      <c r="O24" s="0">
+        <v>17.166561745535713</v>
+      </c>
+      <c r="P24" s="0">
+        <v>2.901596591406459</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K24"/>
+  <dimension ref="A1:J24"/>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="7.26953125" customWidth="true"/>
-    <col min="2" max="2" width="5.7109375" customWidth="true"/>
+    <col min="1" max="1" width="5.7109375" customWidth="true"/>
+    <col min="2" max="2" width="11.7109375" customWidth="true"/>
     <col min="3" max="3" width="11.7109375" customWidth="true"/>
-    <col min="4" max="4" width="11.7109375" customWidth="true"/>
+    <col min="4" max="4" width="13.7109375" customWidth="true"/>
     <col min="5" max="5" width="13.7109375" customWidth="true"/>
     <col min="6" max="6" width="13.7109375" customWidth="true"/>
-    <col min="7" max="7" width="13.7109375" customWidth="true"/>
-    <col min="8" max="8" width="11.7109375" customWidth="true"/>
-    <col min="9" max="9" width="13.7109375" customWidth="true"/>
-    <col min="10" max="10" width="14.37890625" customWidth="true"/>
-    <col min="11" max="11" width="12.7109375" customWidth="true"/>
+    <col min="7" max="7" width="11.7109375" customWidth="true"/>
+    <col min="8" max="8" width="13.7109375" customWidth="true"/>
+    <col min="9" max="9" width="14.37890625" customWidth="true"/>
+    <col min="10" max="10" width="12.7109375" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>183</v>
+        <v>113</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>184</v>
+        <v>114</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>185</v>
+        <v>115</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>186</v>
+        <v>116</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>187</v>
+        <v>117</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>188</v>
+        <v>118</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>189</v>
+        <v>119</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>190</v>
+        <v>120</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>191</v>
+        <v>121</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>192</v>
-      </c>
-      <c r="K1" s="0" t="s">
-        <v>193</v>
+        <v>122</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="0" t="s">
-        <v>194</v>
+        <v>123</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>195</v>
+        <v>124</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>196</v>
+        <v>125</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>197</v>
+        <v>125</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>197</v>
+        <v>125</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>197</v>
+        <v>125</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>197</v>
+        <v>125</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>197</v>
+        <v>125</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>197</v>
+        <v>126</v>
       </c>
       <c r="J2" s="0" t="s">
-        <v>198</v>
-      </c>
-      <c r="K2" s="0" t="s">
-        <v>198</v>
+        <v>126</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="0" t="s">
-        <v>199</v>
+      <c r="A3" s="0">
+        <v>12.190000000000001</v>
       </c>
       <c r="B3" s="0">
-        <v>12.190000000000001</v>
+        <v>201.52877606845385</v>
       </c>
       <c r="C3" s="0">
-        <v>201.52877606845385</v>
+        <v>10.01219720849093</v>
       </c>
       <c r="D3" s="0">
-        <v>10.01219720849093</v>
+        <v>0.14363301630762756</v>
       </c>
       <c r="E3" s="0">
-        <v>0.14363301630762756</v>
+        <v>-0.13250000000000001</v>
       </c>
       <c r="F3" s="0">
-        <v>-0.13250000000000001</v>
+        <v>0.40917600125129522</v>
       </c>
       <c r="G3" s="0">
-        <v>0.40917600125129522</v>
+        <v>3.2324999999999999</v>
       </c>
       <c r="H3" s="0">
-        <v>3.2324999999999999</v>
+        <v>0.395084379173192</v>
       </c>
       <c r="I3" s="0">
-        <v>0.395084379173192</v>
+        <v>0</v>
       </c>
       <c r="J3" s="0">
-        <v>0</v>
-      </c>
-      <c r="K3" s="0">
         <v>1.6367040050051813</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="0" t="s">
-        <v>200</v>
+      <c r="A4" s="0">
+        <v>13.59</v>
       </c>
       <c r="B4" s="0">
-        <v>13.59</v>
+        <v>201.48713504281281</v>
       </c>
       <c r="C4" s="0">
-        <v>201.48713504281281</v>
+        <v>10.24097362914215</v>
       </c>
       <c r="D4" s="0">
-        <v>10.24097362914215</v>
+        <v>0.11547829313839249</v>
       </c>
       <c r="E4" s="0">
-        <v>0.11547829313839249</v>
+        <v>0.37744870533010322</v>
       </c>
       <c r="F4" s="0">
-        <v>0.37744870533010322</v>
+        <v>0.77896182805958314</v>
       </c>
       <c r="G4" s="0">
-        <v>0.77896182805958314</v>
+        <v>3.9028439203513017</v>
       </c>
       <c r="H4" s="0">
-        <v>3.9028439203513017</v>
+        <v>0.50032627388643336</v>
       </c>
       <c r="I4" s="0">
-        <v>0.50032627388643336</v>
+        <v>-2.0397948213204127</v>
       </c>
       <c r="J4" s="0">
-        <v>-2.0397948213204127</v>
-      </c>
-      <c r="K4" s="0">
         <v>3.115847312238333</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="0" t="s">
-        <v>201</v>
+      <c r="A5" s="0">
+        <v>14.59</v>
       </c>
       <c r="B5" s="0">
-        <v>14.59</v>
+        <v>201.45739145306922</v>
       </c>
       <c r="C5" s="0">
-        <v>201.45739145306922</v>
+        <v>9.9763254692479073</v>
       </c>
       <c r="D5" s="0">
-        <v>9.9763254692479073</v>
+        <v>0.10441689371381085</v>
       </c>
       <c r="E5" s="0">
-        <v>0.10441689371381085</v>
+        <v>0.029023622047244513</v>
       </c>
       <c r="F5" s="0">
-        <v>0.029023622047244513</v>
+        <v>0.8017221048052332</v>
       </c>
       <c r="G5" s="0">
+        <v>3.7846929133858254</v>
+      </c>
+      <c r="H5" s="0">
+        <v>0.51925427297230786</v>
+      </c>
+      <c r="I5" s="0">
+        <v>-0.64609448818897786</v>
+      </c>
+      <c r="J5" s="0">
+        <v>3.2068884192209333</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="0">
+        <v>15.02</v>
+      </c>
+      <c r="B6" s="0">
+        <v>201.44482068383846</v>
+      </c>
+      <c r="C6" s="0">
+        <v>10.878138239162579</v>
+      </c>
+      <c r="D6" s="0">
+        <v>0.10350965730875188</v>
+      </c>
+      <c r="E6" s="0">
+        <v>-0.70790171056203965</v>
+      </c>
+      <c r="F6" s="0">
+        <v>0.27775985316468221</v>
+      </c>
+      <c r="G6" s="0">
+        <v>4.5189615802335013</v>
+      </c>
+      <c r="H6" s="0">
+        <v>0.18251895219783656</v>
+      </c>
+      <c r="I6" s="0">
+        <v>2.3016068422481593</v>
+      </c>
+      <c r="J6" s="0">
+        <v>1.1110394126587284</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="0">
+        <v>15.289999999999999</v>
+      </c>
+      <c r="B7" s="0">
+        <v>201.43974606845384</v>
+      </c>
+      <c r="C7" s="0">
+        <v>9.8872299810538102</v>
+      </c>
+      <c r="D7" s="0">
+        <v>0.10382787734144472</v>
+      </c>
+      <c r="E7" s="0">
+        <v>-0.8601732283464566</v>
+      </c>
+      <c r="F7" s="0">
+        <v>0.76956930410023416</v>
+      </c>
+      <c r="G7" s="0">
+        <v>3.7317440944881897</v>
+      </c>
+      <c r="H7" s="0">
+        <v>0.49856927291608044</v>
+      </c>
+      <c r="I7" s="0">
+        <v>2.9106929133858275</v>
+      </c>
+      <c r="J7" s="0">
+        <v>3.0782772164009371</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="0">
+        <v>15.640000000000001</v>
+      </c>
+      <c r="B8" s="0">
+        <v>201.43316786332562</v>
+      </c>
+      <c r="C8" s="0">
+        <v>10.708374995046363</v>
+      </c>
+      <c r="D8" s="0">
+        <v>0.10475773652306104</v>
+      </c>
+      <c r="E8" s="0">
+        <v>-0.71741309775302509</v>
+      </c>
+      <c r="F8" s="0">
+        <v>0.33941517159654622</v>
+      </c>
+      <c r="G8" s="0">
+        <v>3.7449907176237112</v>
+      </c>
+      <c r="H8" s="0">
+        <v>0.44666202463959798</v>
+      </c>
+      <c r="I8" s="0">
+        <v>2.3396523910121005</v>
+      </c>
+      <c r="J8" s="0">
+        <v>1.3576606863861855</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="0">
+        <v>15.940000000000001</v>
+      </c>
+      <c r="B9" s="0">
+        <v>201.42752940178718</v>
+      </c>
+      <c r="C9" s="0">
+        <v>11.039549024903264</v>
+      </c>
+      <c r="D9" s="0">
+        <v>0.097150894309145294</v>
+      </c>
+      <c r="E9" s="0">
+        <v>0.063700787401571451</v>
+      </c>
+      <c r="F9" s="0">
         <v>0.8017221048052332</v>
       </c>
-      <c r="H5" s="0">
-        <v>3.7846929133858254</v>
-      </c>
-      <c r="I5" s="0">
+      <c r="G9" s="0">
+        <v>4.077391304347822</v>
+      </c>
+      <c r="H9" s="0">
         <v>0.51925427297230786</v>
       </c>
-      <c r="J5" s="0">
-        <v>-0.64609448818897786</v>
-      </c>
-      <c r="K5" s="0">
+      <c r="I9" s="0">
+        <v>-0.78480314960628594</v>
+      </c>
+      <c r="J9" s="0">
         <v>3.2068884192209333</v>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" s="0" t="s">
-        <v>202</v>
-      </c>
-      <c r="B6" s="0">
-        <v>15.02</v>
-      </c>
-      <c r="C6" s="0">
-        <v>201.44482068383846</v>
-      </c>
-      <c r="D6" s="0">
-        <v>10.878138239162579</v>
-      </c>
-      <c r="E6" s="0">
-        <v>0.10350965730875188</v>
-      </c>
-      <c r="F6" s="0">
-        <v>-0.70790171056203965</v>
-      </c>
-      <c r="G6" s="0">
-        <v>0.27775985316468221</v>
-      </c>
-      <c r="H6" s="0">
-        <v>4.5189615802335013</v>
-      </c>
-      <c r="I6" s="0">
-        <v>0.18251895219783656</v>
-      </c>
-      <c r="J6" s="0">
-        <v>2.3016068422481593</v>
-      </c>
-      <c r="K6" s="0">
-        <v>1.1110394126587284</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="0" t="s">
-        <v>203</v>
-      </c>
-      <c r="B7" s="0">
-        <v>15.289999999999999</v>
-      </c>
-      <c r="C7" s="0">
-        <v>201.43974606845384</v>
-      </c>
-      <c r="D7" s="0">
-        <v>9.8872299810538102</v>
-      </c>
-      <c r="E7" s="0">
-        <v>0.10382787734144472</v>
-      </c>
-      <c r="F7" s="0">
-        <v>-0.8601732283464566</v>
-      </c>
-      <c r="G7" s="0">
-        <v>0.76956930410023416</v>
-      </c>
-      <c r="H7" s="0">
-        <v>3.7317440944881897</v>
-      </c>
-      <c r="I7" s="0">
-        <v>0.49856927291608044</v>
-      </c>
-      <c r="J7" s="0">
-        <v>2.9106929133858275</v>
-      </c>
-      <c r="K7" s="0">
-        <v>3.0782772164009371</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="0" t="s">
-        <v>204</v>
-      </c>
-      <c r="B8" s="0">
-        <v>15.640000000000001</v>
-      </c>
-      <c r="C8" s="0">
-        <v>201.43316786332562</v>
-      </c>
-      <c r="D8" s="0">
-        <v>10.708374995046363</v>
-      </c>
-      <c r="E8" s="0">
-        <v>0.10475773652306104</v>
-      </c>
-      <c r="F8" s="0">
-        <v>-0.71741309775302509</v>
-      </c>
-      <c r="G8" s="0">
-        <v>0.33941517159654622</v>
-      </c>
-      <c r="H8" s="0">
-        <v>3.7449907176237112</v>
-      </c>
-      <c r="I8" s="0">
-        <v>0.44666202463959798</v>
-      </c>
-      <c r="J8" s="0">
-        <v>2.3396523910121005</v>
-      </c>
-      <c r="K8" s="0">
-        <v>1.3576606863861855</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="0" t="s">
-        <v>205</v>
-      </c>
-      <c r="B9" s="0">
-        <v>15.940000000000001</v>
-      </c>
-      <c r="C9" s="0">
-        <v>201.42752940178718</v>
-      </c>
-      <c r="D9" s="0">
-        <v>11.039549024903264</v>
-      </c>
-      <c r="E9" s="0">
-        <v>0.097150894309145294</v>
-      </c>
-      <c r="F9" s="0">
-        <v>0.063700787401571451</v>
-      </c>
-      <c r="G9" s="0">
+    <row r="10">
+      <c r="A10" s="0">
+        <v>16.190000000000001</v>
+      </c>
+      <c r="B10" s="0">
+        <v>201.42283068383844</v>
+      </c>
+      <c r="C10" s="0">
+        <v>10.762272249201416</v>
+      </c>
+      <c r="D10" s="0">
+        <v>0.088684907140420544</v>
+      </c>
+      <c r="E10" s="0">
+        <v>-1.1603550878255602</v>
+      </c>
+      <c r="F10" s="0">
+        <v>0.042883263899249804</v>
+      </c>
+      <c r="G10" s="0">
+        <v>3.3930330102967901</v>
+      </c>
+      <c r="H10" s="0">
+        <v>0.11008374535465781</v>
+      </c>
+      <c r="I10" s="0">
+        <v>4.1114203513022414</v>
+      </c>
+      <c r="J10" s="0">
+        <v>0.1715330555969995</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="0">
+        <v>16.539999999999999</v>
+      </c>
+      <c r="B11" s="0">
+        <v>201.41625247871025</v>
+      </c>
+      <c r="C11" s="0">
+        <v>10.835984879209818</v>
+      </c>
+      <c r="D11" s="0">
+        <v>0.10998966327131669</v>
+      </c>
+      <c r="E11" s="0">
+        <v>-0.63608858267716772</v>
+      </c>
+      <c r="F11" s="0">
+        <v>0.57102014147248525</v>
+      </c>
+      <c r="G11" s="0">
+        <v>3.2646003937007873</v>
+      </c>
+      <c r="H11" s="0">
+        <v>0.40554424135375533</v>
+      </c>
+      <c r="I11" s="0">
+        <v>2.0143543307086711</v>
+      </c>
+      <c r="J11" s="0">
+        <v>2.2840805658899415</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="0">
+        <v>16.890000000000001</v>
+      </c>
+      <c r="B12" s="0">
+        <v>201.40967427358206</v>
+      </c>
+      <c r="C12" s="0">
+        <v>10.459512485805641</v>
+      </c>
+      <c r="D12" s="0">
+        <v>0.11454452430566182</v>
+      </c>
+      <c r="E12" s="0">
+        <v>-0.11602362204725768</v>
+      </c>
+      <c r="F12" s="0">
+        <v>0.26972275316592836</v>
+      </c>
+      <c r="G12" s="0">
+        <v>3.4375554760200258</v>
+      </c>
+      <c r="H12" s="0">
+        <v>0.026115763878443478</v>
+      </c>
+      <c r="I12" s="0">
+        <v>-0.065905511810969764</v>
+      </c>
+      <c r="J12" s="0">
+        <v>1.0788910126637137</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="0">
+        <v>17.120000000000001</v>
+      </c>
+      <c r="B13" s="0">
+        <v>201.40535145306922</v>
+      </c>
+      <c r="C13" s="0">
+        <v>10.384159531398856</v>
+      </c>
+      <c r="D13" s="0">
+        <v>0.11901469625718146</v>
+      </c>
+      <c r="E13" s="0">
+        <v>-0.64282955071792613</v>
+      </c>
+      <c r="F13" s="0">
+        <v>0.057459940335953731</v>
+      </c>
+      <c r="G13" s="0">
+        <v>2.9475636868920798</v>
+      </c>
+      <c r="H13" s="0">
+        <v>0.13920006295401072</v>
+      </c>
+      <c r="I13" s="0">
+        <v>2.0413182028717043</v>
+      </c>
+      <c r="J13" s="0">
+        <v>0.2298397613438149</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="0">
+        <v>17.490000000000002</v>
+      </c>
+      <c r="B14" s="0">
+        <v>201.39839735050512</v>
+      </c>
+      <c r="C14" s="0">
+        <v>9.9436806178566286</v>
+      </c>
+      <c r="D14" s="0">
+        <v>0.096262499948600366</v>
+      </c>
+      <c r="E14" s="0">
+        <v>-0.98800293345685053</v>
+      </c>
+      <c r="F14" s="0">
+        <v>0.08750534568451096</v>
+      </c>
+      <c r="G14" s="0">
+        <v>2.9854948278524009</v>
+      </c>
+      <c r="H14" s="0">
+        <v>0.11011667130346764</v>
+      </c>
+      <c r="I14" s="0">
+        <v>3.4220117338274001</v>
+      </c>
+      <c r="J14" s="0">
+        <v>0.35002138273804345</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="0">
+        <v>18.210000000000001</v>
+      </c>
+      <c r="B15" s="0">
+        <v>201.38486504281281</v>
+      </c>
+      <c r="C15" s="0">
+        <v>9.9960501404771449</v>
+      </c>
+      <c r="D15" s="0">
+        <v>0.10589632985968327</v>
+      </c>
+      <c r="E15" s="0">
+        <v>-0.72329651716043897</v>
+      </c>
+      <c r="F15" s="0">
+        <v>0.7342202138225592</v>
+      </c>
+      <c r="G15" s="0">
+        <v>2.4119468375309268</v>
+      </c>
+      <c r="H15" s="0">
+        <v>0.49269297196336881</v>
+      </c>
+      <c r="I15" s="0">
+        <v>2.3631860686417565</v>
+      </c>
+      <c r="J15" s="0">
+        <v>2.9368808552902372</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="0">
+        <v>18.439999999999998</v>
+      </c>
+      <c r="B16" s="0">
+        <v>201.38054222229999</v>
+      </c>
+      <c r="C16" s="0">
+        <v>8.9507559822158029</v>
+      </c>
+      <c r="D16" s="0">
+        <v>0.20756565956142378</v>
+      </c>
+      <c r="E16" s="0">
+        <v>-0.76907473196726461</v>
+      </c>
+      <c r="F16" s="0">
+        <v>0.6414142290289524</v>
+      </c>
+      <c r="G16" s="0">
+        <v>2.3596288777516983</v>
+      </c>
+      <c r="H16" s="0">
+        <v>0.45617476985601274</v>
+      </c>
+      <c r="I16" s="0">
+        <v>2.5462989278690591</v>
+      </c>
+      <c r="J16" s="0">
+        <v>2.5656569161158091</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="0">
+        <v>18.84</v>
+      </c>
+      <c r="B17" s="0">
+        <v>201.37302427358205</v>
+      </c>
+      <c r="C17" s="0">
+        <v>9.2453681244467258</v>
+      </c>
+      <c r="D17" s="0">
+        <v>0.1085995457562766</v>
+      </c>
+      <c r="E17" s="0">
+        <v>-0.84868901858783219</v>
+      </c>
+      <c r="F17" s="0">
+        <v>0.48001251634441555</v>
+      </c>
+      <c r="G17" s="0">
+        <v>2.2686411216139062</v>
+      </c>
+      <c r="H17" s="0">
+        <v>0.39266485314756605</v>
+      </c>
+      <c r="I17" s="0">
+        <v>2.8647560743513294</v>
+      </c>
+      <c r="J17" s="0">
+        <v>1.9200500653776615</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="0">
+        <v>20.140000000000001</v>
+      </c>
+      <c r="B18" s="0">
+        <v>201.34857658127436</v>
+      </c>
+      <c r="C18" s="0">
+        <v>8.1044394762742993</v>
+      </c>
+      <c r="D18" s="0">
+        <v>0.11800414700884421</v>
+      </c>
+      <c r="E18" s="0">
+        <v>-1.7484999999999999</v>
+      </c>
+      <c r="F18" s="0">
         <v>0.8017221048052332</v>
       </c>
-      <c r="H9" s="0">
-        <v>4.077391304347822</v>
-      </c>
-      <c r="I9" s="0">
+      <c r="G18" s="0">
+        <v>2.0686249999999999</v>
+      </c>
+      <c r="H18" s="0">
         <v>0.51925427297230786</v>
       </c>
-      <c r="J9" s="0">
-        <v>-0.78480314960628594</v>
-      </c>
-      <c r="K9" s="0">
+      <c r="I18" s="0">
+        <v>6.4640000000000022</v>
+      </c>
+      <c r="J18" s="0">
         <v>3.2068884192209333</v>
       </c>
     </row>
-    <row r="10">
-      <c r="A10" s="0" t="s">
-        <v>206</v>
-      </c>
-      <c r="B10" s="0">
-        <v>16.190000000000001</v>
-      </c>
-      <c r="C10" s="0">
-        <v>201.42283068383844</v>
-      </c>
-      <c r="D10" s="0">
-        <v>10.762272249201416</v>
-      </c>
-      <c r="E10" s="0">
-        <v>0.088684907140420544</v>
-      </c>
-      <c r="F10" s="0">
-        <v>-1.1603550878255602</v>
-      </c>
-      <c r="G10" s="0">
-        <v>0.042883263899249804</v>
-      </c>
-      <c r="H10" s="0">
-        <v>3.3930330102967901</v>
-      </c>
-      <c r="I10" s="0">
-        <v>0.11008374535465781</v>
-      </c>
-      <c r="J10" s="0">
-        <v>4.1114203513022414</v>
-      </c>
-      <c r="K10" s="0">
-        <v>0.1715330555969995</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="0" t="s">
-        <v>207</v>
-      </c>
-      <c r="B11" s="0">
-        <v>16.539999999999999</v>
-      </c>
-      <c r="C11" s="0">
-        <v>201.41625247871025</v>
-      </c>
-      <c r="D11" s="0">
-        <v>10.835984879209818</v>
-      </c>
-      <c r="E11" s="0">
-        <v>0.10998966327131669</v>
-      </c>
-      <c r="F11" s="0">
-        <v>-0.63608858267716772</v>
-      </c>
-      <c r="G11" s="0">
-        <v>0.57102014147248525</v>
-      </c>
-      <c r="H11" s="0">
-        <v>3.2646003937007873</v>
-      </c>
-      <c r="I11" s="0">
-        <v>0.40554424135375533</v>
-      </c>
-      <c r="J11" s="0">
-        <v>2.0143543307086711</v>
-      </c>
-      <c r="K11" s="0">
-        <v>2.2840805658899415</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="0" t="s">
-        <v>208</v>
-      </c>
-      <c r="B12" s="0">
-        <v>16.890000000000001</v>
-      </c>
-      <c r="C12" s="0">
-        <v>201.40967427358206</v>
-      </c>
-      <c r="D12" s="0">
-        <v>10.459512485805641</v>
-      </c>
-      <c r="E12" s="0">
-        <v>0.11454452430566182</v>
-      </c>
-      <c r="F12" s="0">
-        <v>-0.11602362204725768</v>
-      </c>
-      <c r="G12" s="0">
-        <v>0.26972275316592836</v>
-      </c>
-      <c r="H12" s="0">
-        <v>3.4375554760200258</v>
-      </c>
-      <c r="I12" s="0">
-        <v>0.026115763878443478</v>
-      </c>
-      <c r="J12" s="0">
-        <v>-0.065905511810969764</v>
-      </c>
-      <c r="K12" s="0">
-        <v>1.0788910126637137</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="0" t="s">
-        <v>209</v>
-      </c>
-      <c r="B13" s="0">
-        <v>17.120000000000001</v>
-      </c>
-      <c r="C13" s="0">
-        <v>201.40535145306922</v>
-      </c>
-      <c r="D13" s="0">
-        <v>10.384159531398856</v>
-      </c>
-      <c r="E13" s="0">
-        <v>0.11901469625718146</v>
-      </c>
-      <c r="F13" s="0">
-        <v>-0.64282955071792613</v>
-      </c>
-      <c r="G13" s="0">
-        <v>0.057459940335953731</v>
-      </c>
-      <c r="H13" s="0">
-        <v>2.9475636868920798</v>
-      </c>
-      <c r="I13" s="0">
-        <v>0.13920006295401072</v>
-      </c>
-      <c r="J13" s="0">
-        <v>2.0413182028717043</v>
-      </c>
-      <c r="K13" s="0">
-        <v>0.2298397613438149</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="0" t="s">
-        <v>210</v>
-      </c>
-      <c r="B14" s="0">
-        <v>17.490000000000002</v>
-      </c>
-      <c r="C14" s="0">
-        <v>201.39839735050512</v>
-      </c>
-      <c r="D14" s="0">
-        <v>9.9436806178566286</v>
-      </c>
-      <c r="E14" s="0">
-        <v>0.096262499948600366</v>
-      </c>
-      <c r="F14" s="0">
-        <v>-0.98800293345685053</v>
-      </c>
-      <c r="G14" s="0">
-        <v>0.08750534568451096</v>
-      </c>
-      <c r="H14" s="0">
-        <v>2.9854948278524009</v>
-      </c>
-      <c r="I14" s="0">
-        <v>0.11011667130346764</v>
-      </c>
-      <c r="J14" s="0">
-        <v>3.4220117338274001</v>
-      </c>
-      <c r="K14" s="0">
-        <v>0.35002138273804345</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" s="0" t="s">
-        <v>211</v>
-      </c>
-      <c r="B15" s="0">
-        <v>18.210000000000001</v>
-      </c>
-      <c r="C15" s="0">
-        <v>201.38486504281281</v>
-      </c>
-      <c r="D15" s="0">
-        <v>9.9960501404771449</v>
-      </c>
-      <c r="E15" s="0">
-        <v>0.10589632985968327</v>
-      </c>
-      <c r="F15" s="0">
-        <v>-0.72329651716043897</v>
-      </c>
-      <c r="G15" s="0">
-        <v>0.7342202138225592</v>
-      </c>
-      <c r="H15" s="0">
-        <v>2.4119468375309268</v>
-      </c>
-      <c r="I15" s="0">
-        <v>0.49269297196336881</v>
-      </c>
-      <c r="J15" s="0">
-        <v>2.3631860686417565</v>
-      </c>
-      <c r="K15" s="0">
-        <v>2.9368808552902372</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="0" t="s">
-        <v>212</v>
-      </c>
-      <c r="B16" s="0">
-        <v>18.439999999999998</v>
-      </c>
-      <c r="C16" s="0">
-        <v>201.38054222229999</v>
-      </c>
-      <c r="D16" s="0">
-        <v>8.9507559822158029</v>
-      </c>
-      <c r="E16" s="0">
-        <v>0.20756565956142378</v>
-      </c>
-      <c r="F16" s="0">
-        <v>-0.76907473196726461</v>
-      </c>
-      <c r="G16" s="0">
-        <v>0.6414142290289524</v>
-      </c>
-      <c r="H16" s="0">
-        <v>2.3596288777516983</v>
-      </c>
-      <c r="I16" s="0">
-        <v>0.45617476985601274</v>
-      </c>
-      <c r="J16" s="0">
-        <v>2.5462989278690591</v>
-      </c>
-      <c r="K16" s="0">
-        <v>2.5656569161158091</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" s="0" t="s">
-        <v>213</v>
-      </c>
-      <c r="B17" s="0">
-        <v>18.84</v>
-      </c>
-      <c r="C17" s="0">
-        <v>201.37302427358205</v>
-      </c>
-      <c r="D17" s="0">
-        <v>9.2453681244467258</v>
-      </c>
-      <c r="E17" s="0">
-        <v>0.1085995457562766</v>
-      </c>
-      <c r="F17" s="0">
-        <v>-0.84868901858783219</v>
-      </c>
-      <c r="G17" s="0">
-        <v>0.48001251634441555</v>
-      </c>
-      <c r="H17" s="0">
-        <v>2.2686411216139062</v>
-      </c>
-      <c r="I17" s="0">
-        <v>0.39266485314756605</v>
-      </c>
-      <c r="J17" s="0">
-        <v>2.8647560743513294</v>
-      </c>
-      <c r="K17" s="0">
-        <v>1.9200500653776615</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" s="0" t="s">
-        <v>214</v>
-      </c>
-      <c r="B18" s="0">
-        <v>20.140000000000001</v>
-      </c>
-      <c r="C18" s="0">
-        <v>201.34857658127436</v>
-      </c>
-      <c r="D18" s="0">
-        <v>8.1044394762742993</v>
-      </c>
-      <c r="E18" s="0">
-        <v>0.11800414700884421</v>
-      </c>
-      <c r="F18" s="0">
-        <v>-1.7484999999999999</v>
-      </c>
-      <c r="G18" s="0">
+    <row r="19">
+      <c r="A19" s="0">
+        <v>20.640000000000001</v>
+      </c>
+      <c r="B19" s="0">
+        <v>201.33912786332564</v>
+      </c>
+      <c r="C19" s="0">
+        <v>9.7067607134899703</v>
+      </c>
+      <c r="D19" s="0">
+        <v>0.10902200739197236</v>
+      </c>
+      <c r="E19" s="0">
+        <v>-0.85450000000000126</v>
+      </c>
+      <c r="F19" s="0">
+        <v>0.68732639542481855</v>
+      </c>
+      <c r="G19" s="0">
+        <v>1.8960285714285714</v>
+      </c>
+      <c r="H19" s="0">
+        <v>0.2972487690582083</v>
+      </c>
+      <c r="I19" s="0">
+        <v>2.8880000000000048</v>
+      </c>
+      <c r="J19" s="0">
+        <v>2.7493055816992737</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="0">
+        <v>21.120000000000001</v>
+      </c>
+      <c r="B20" s="0">
+        <v>201.33005709409485</v>
+      </c>
+      <c r="C20" s="0">
+        <v>8.4942813608424057</v>
+      </c>
+      <c r="D20" s="0">
+        <v>0.10853455716108885</v>
+      </c>
+      <c r="E20" s="0">
+        <v>-0.67841044776119386</v>
+      </c>
+      <c r="F20" s="0">
+        <v>0.54644398504411484</v>
+      </c>
+      <c r="G20" s="0">
+        <v>1.8858228855721393</v>
+      </c>
+      <c r="H20" s="0">
+        <v>0.26850920262175043</v>
+      </c>
+      <c r="I20" s="0">
+        <v>2.1836417910447752</v>
+      </c>
+      <c r="J20" s="0">
+        <v>2.1857759401764585</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="0">
+        <v>21.140000000000001</v>
+      </c>
+      <c r="B21" s="0">
+        <v>201.32967914537693</v>
+      </c>
+      <c r="C21" s="0">
+        <v>6.9697748282639225</v>
+      </c>
+      <c r="D21" s="0">
+        <v>0.087536853144447743</v>
+      </c>
+      <c r="E21" s="0">
+        <v>-0.68929104477611902</v>
+      </c>
+      <c r="F21" s="0">
+        <v>0.539983748256045</v>
+      </c>
+      <c r="G21" s="0">
+        <v>1.887542288557214</v>
+      </c>
+      <c r="H21" s="0">
+        <v>0.27226304613143282</v>
+      </c>
+      <c r="I21" s="0">
+        <v>2.2271641791044763</v>
+      </c>
+      <c r="J21" s="0">
+        <v>2.1599349930241791</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="0">
+        <v>23.539999999999999</v>
+      </c>
+      <c r="B22" s="0">
+        <v>201.28432529922307</v>
+      </c>
+      <c r="C22" s="0">
+        <v>7.1065964233074652</v>
+      </c>
+      <c r="D22" s="0">
+        <v>0.095202654485499486</v>
+      </c>
+      <c r="E22" s="0">
+        <v>-1.513714285714286</v>
+      </c>
+      <c r="F22" s="0">
         <v>0.8017221048052332</v>
       </c>
-      <c r="H18" s="0">
-        <v>2.0686249999999999</v>
-      </c>
-      <c r="I18" s="0">
+      <c r="G22" s="0">
+        <v>2.722</v>
+      </c>
+      <c r="H22" s="0">
         <v>0.51925427297230786</v>
       </c>
-      <c r="J18" s="0">
-        <v>6.4640000000000022</v>
-      </c>
-      <c r="K18" s="0">
+      <c r="I22" s="0">
+        <v>5.524857142857142</v>
+      </c>
+      <c r="J22" s="0">
         <v>3.2068884192209333</v>
       </c>
     </row>
-    <row r="19">
-      <c r="A19" s="0" t="s">
-        <v>215</v>
-      </c>
-      <c r="B19" s="0">
-        <v>20.640000000000001</v>
-      </c>
-      <c r="C19" s="0">
-        <v>201.33912786332564</v>
-      </c>
-      <c r="D19" s="0">
-        <v>9.7067607134899703</v>
-      </c>
-      <c r="E19" s="0">
-        <v>0.10902200739197236</v>
-      </c>
-      <c r="F19" s="0">
-        <v>-0.85450000000000126</v>
-      </c>
-      <c r="G19" s="0">
-        <v>0.68732639542481855</v>
-      </c>
-      <c r="H19" s="0">
-        <v>1.8960285714285714</v>
-      </c>
-      <c r="I19" s="0">
-        <v>0.2972487690582083</v>
-      </c>
-      <c r="J19" s="0">
-        <v>2.8880000000000048</v>
-      </c>
-      <c r="K19" s="0">
-        <v>2.7493055816992737</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" s="0" t="s">
-        <v>216</v>
-      </c>
-      <c r="B20" s="0">
-        <v>21.120000000000001</v>
-      </c>
-      <c r="C20" s="0">
-        <v>201.33005709409485</v>
-      </c>
-      <c r="D20" s="0">
-        <v>8.4942813608424057</v>
-      </c>
-      <c r="E20" s="0">
-        <v>0.10853455716108885</v>
-      </c>
-      <c r="F20" s="0">
-        <v>-0.67841044776119386</v>
-      </c>
-      <c r="G20" s="0">
-        <v>0.54644398504411484</v>
-      </c>
-      <c r="H20" s="0">
-        <v>1.8858228855721393</v>
-      </c>
-      <c r="I20" s="0">
-        <v>0.26850920262175043</v>
-      </c>
-      <c r="J20" s="0">
-        <v>2.1836417910447752</v>
-      </c>
-      <c r="K20" s="0">
-        <v>2.1857759401764585</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" s="0" t="s">
-        <v>217</v>
-      </c>
-      <c r="B21" s="0">
-        <v>21.140000000000001</v>
-      </c>
-      <c r="C21" s="0">
-        <v>201.32967914537693</v>
-      </c>
-      <c r="D21" s="0">
-        <v>6.9697748282639225</v>
-      </c>
-      <c r="E21" s="0">
-        <v>0.087536853144447743</v>
-      </c>
-      <c r="F21" s="0">
-        <v>-0.68929104477611902</v>
-      </c>
-      <c r="G21" s="0">
-        <v>0.539983748256045</v>
-      </c>
-      <c r="H21" s="0">
-        <v>1.887542288557214</v>
-      </c>
-      <c r="I21" s="0">
-        <v>0.27226304613143282</v>
-      </c>
-      <c r="J21" s="0">
-        <v>2.2271641791044763</v>
-      </c>
-      <c r="K21" s="0">
-        <v>2.1599349930241791</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" s="0" t="s">
-        <v>218</v>
-      </c>
-      <c r="B22" s="0">
-        <v>23.539999999999999</v>
-      </c>
-      <c r="C22" s="0">
-        <v>201.28432529922307</v>
-      </c>
-      <c r="D22" s="0">
-        <v>7.1065964233074652</v>
-      </c>
-      <c r="E22" s="0">
-        <v>0.095202654485499486</v>
-      </c>
-      <c r="F22" s="0">
-        <v>-1.513714285714286</v>
-      </c>
-      <c r="G22" s="0">
+    <row r="23">
+      <c r="A23" s="0">
+        <v>23.890000000000001</v>
+      </c>
+      <c r="B23" s="0">
+        <v>201.27771119665897</v>
+      </c>
+      <c r="C23" s="0">
+        <v>9.3714561608127696</v>
+      </c>
+      <c r="D23" s="0">
+        <v>0.12036219998484181</v>
+      </c>
+      <c r="E23" s="0">
+        <v>-1.4951517857142858</v>
+      </c>
+      <c r="F23" s="0">
         <v>0.8017221048052332</v>
       </c>
-      <c r="H22" s="0">
-        <v>2.722</v>
-      </c>
-      <c r="I22" s="0">
+      <c r="G23" s="0">
+        <v>2.698375</v>
+      </c>
+      <c r="H23" s="0">
         <v>0.51925427297230786</v>
       </c>
-      <c r="J22" s="0">
-        <v>5.524857142857142</v>
-      </c>
-      <c r="K22" s="0">
+      <c r="I23" s="0">
+        <v>5.4506071428571419</v>
+      </c>
+      <c r="J23" s="0">
         <v>3.2068884192209333</v>
       </c>
     </row>
-    <row r="23">
-      <c r="A23" s="0" t="s">
-        <v>219</v>
-      </c>
-      <c r="B23" s="0">
-        <v>23.890000000000001</v>
-      </c>
-      <c r="C23" s="0">
-        <v>201.27771119665897</v>
-      </c>
-      <c r="D23" s="0">
-        <v>9.3714561608127696</v>
-      </c>
-      <c r="E23" s="0">
-        <v>0.12036219998484181</v>
-      </c>
-      <c r="F23" s="0">
-        <v>-1.4951517857142858</v>
-      </c>
-      <c r="G23" s="0">
+    <row r="24">
+      <c r="A24" s="0">
+        <v>24.189999999999998</v>
+      </c>
+      <c r="B24" s="0">
+        <v>201.27204196588974</v>
+      </c>
+      <c r="C24" s="0">
+        <v>9.5039834385630684</v>
+      </c>
+      <c r="D24" s="0">
+        <v>0.11997061322388737</v>
+      </c>
+      <c r="E24" s="0">
+        <v>-1.4792410714285715</v>
+      </c>
+      <c r="F24" s="0">
         <v>0.8017221048052332</v>
       </c>
-      <c r="H23" s="0">
-        <v>2.698375</v>
-      </c>
-      <c r="I23" s="0">
+      <c r="G24" s="0">
+        <v>2.6781250000000001</v>
+      </c>
+      <c r="H24" s="0">
         <v>0.51925427297230786</v>
       </c>
-      <c r="J23" s="0">
-        <v>5.4506071428571419</v>
-      </c>
-      <c r="K23" s="0">
-        <v>3.2068884192209333</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" s="0" t="s">
-        <v>220</v>
-      </c>
-      <c r="B24" s="0">
-        <v>24.189999999999998</v>
-      </c>
-      <c r="C24" s="0">
-        <v>201.27204196588974</v>
-      </c>
-      <c r="D24" s="0">
-        <v>9.5039834385630684</v>
-      </c>
-      <c r="E24" s="0">
-        <v>0.11997061322388737</v>
-      </c>
-      <c r="F24" s="0">
-        <v>-1.4792410714285715</v>
-      </c>
-      <c r="G24" s="0">
-        <v>0.8017221048052332</v>
-      </c>
-      <c r="H24" s="0">
-        <v>2.6781250000000001</v>
-      </c>
       <c r="I24" s="0">
-        <v>0.51925427297230786</v>
+        <v>5.3869642857142859</v>
       </c>
       <c r="J24" s="0">
-        <v>5.3869642857142859</v>
-      </c>
-      <c r="K24" s="0">
         <v>3.2068884192209333</v>
       </c>
     </row>
@@ -3481,12 +4406,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A0F56654C37D7A4AAC59B6C288F9CE16" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="563f837eafd1d134d0191c976a557f73">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="7fa73a2b-a877-44bc-b864-c31a95c8f621" xmlns:ns4="4bb6f66d-1447-4ffa-a850-4f1b35540af2" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9f764ae2895bc9eb9b73becb11c151bc" ns3:_="" ns4:_="">
     <xsd:import namespace="7fa73a2b-a877-44bc-b864-c31a95c8f621"/>
@@ -3709,7 +4628,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -3718,16 +4637,13 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{45DDE364-39F5-4CB5-B004-A75D4718A354}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8F8399FD-C108-4E5D-8E4F-378098980073}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3746,10 +4662,19 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{48B0DCBC-551C-4D59-922B-DAF738475938}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{45DDE364-39F5-4CB5-B004-A75D4718A354}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>